<commit_message>
EPBDS-8508 added one more test
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8508.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8508.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvlad\.openl-webstudio\user-workspace\DEFAULT\EPBDS-8508\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797F4401-90FB-4BAE-BEA8-3D7E75DA88B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F126D94-8073-41BE-9A70-95C3E354D26E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="132">
   <si>
     <t>String</t>
   </si>
@@ -356,6 +356,66 @@
   </si>
   <si>
     <t>_description_</t>
+  </si>
+  <si>
+    <t>SmartRules String group2(String input1, String input2, String input3, Integer input4)</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>1.. 3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>4.. 6</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>7 ..9</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>9 .. 10</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>&lt; 22</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>&gt; 22</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>Test group2</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -513,14 +573,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -860,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:AA58"/>
+  <dimension ref="B6:AA91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -878,34 +938,34 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:27" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
     </row>
     <row r="7" spans="2:27" s="1" customFormat="1">
       <c r="B7" s="2" t="s">
@@ -983,7 +1043,7 @@
       <c r="Z7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AA7" s="12" t="s">
+      <c r="AA7" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2736,6 +2796,280 @@
         <v>99</v>
       </c>
     </row>
+    <row r="71" spans="2:6">
+      <c r="B71" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" t="s">
+        <v>114</v>
+      </c>
+      <c r="E73" t="s">
+        <v>115</v>
+      </c>
+      <c r="F73" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" t="s">
+        <v>117</v>
+      </c>
+      <c r="C74" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" t="s">
+        <v>114</v>
+      </c>
+      <c r="E74" t="s">
+        <v>118</v>
+      </c>
+      <c r="F74" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" t="s">
+        <v>114</v>
+      </c>
+      <c r="E75" t="s">
+        <v>121</v>
+      </c>
+      <c r="F75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="C76" t="s">
+        <v>117</v>
+      </c>
+      <c r="D76" t="s">
+        <v>117</v>
+      </c>
+      <c r="E76" t="s">
+        <v>123</v>
+      </c>
+      <c r="F76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="D77" t="s">
+        <v>117</v>
+      </c>
+      <c r="E77" t="s">
+        <v>125</v>
+      </c>
+      <c r="F77" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="E78" t="s">
+        <v>127</v>
+      </c>
+      <c r="F78" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="B80" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s">
+        <v>3</v>
+      </c>
+      <c r="E82" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" t="s">
+        <v>114</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" t="s">
+        <v>114</v>
+      </c>
+      <c r="D84" t="s">
+        <v>114</v>
+      </c>
+      <c r="E84">
+        <v>5</v>
+      </c>
+      <c r="F84" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6">
+      <c r="B85" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85" t="s">
+        <v>120</v>
+      </c>
+      <c r="D85" t="s">
+        <v>114</v>
+      </c>
+      <c r="E85">
+        <v>8</v>
+      </c>
+      <c r="F85" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="C86" t="s">
+        <v>117</v>
+      </c>
+      <c r="D86" t="s">
+        <v>117</v>
+      </c>
+      <c r="E86">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6">
+      <c r="D87" t="s">
+        <v>117</v>
+      </c>
+      <c r="E87">
+        <v>11</v>
+      </c>
+      <c r="F87" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="E88">
+        <v>44</v>
+      </c>
+      <c r="F88" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6">
+      <c r="B89" t="s">
+        <v>130</v>
+      </c>
+      <c r="C89" t="s">
+        <v>130</v>
+      </c>
+      <c r="D89" t="s">
+        <v>131</v>
+      </c>
+      <c r="E89">
+        <v>44</v>
+      </c>
+      <c r="F89" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6">
+      <c r="B90" t="s">
+        <v>130</v>
+      </c>
+      <c r="C90" t="s">
+        <v>130</v>
+      </c>
+      <c r="D90" t="s">
+        <v>117</v>
+      </c>
+      <c r="E90">
+        <v>11</v>
+      </c>
+      <c r="F90" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6">
+      <c r="B91" t="s">
+        <v>130</v>
+      </c>
+      <c r="C91" t="s">
+        <v>117</v>
+      </c>
+      <c r="D91" t="s">
+        <v>117</v>
+      </c>
+      <c r="E91">
+        <v>9</v>
+      </c>
+      <c r="F91" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B6:AA6"/>

</xml_diff>